<commit_message>
update 2 from second ITI Tech virtual-face-to-face session
</commit_message>
<xml_diff>
--- a/MHDS/MHDS-Comment-Second.xlsx
+++ b/MHDS/MHDS-Comment-Second.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\john.moehrke\Git\IT-Infrastructure\MHDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28E8100-EA90-49A7-B220-A6867EB6AF3A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92074ABD-B272-4772-8735-A482FE49BC99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="232">
   <si>
     <t>Priority</t>
   </si>
@@ -2960,27 +2960,6 @@
     <t>move to closed</t>
   </si>
   <si>
-    <t>Is there a need to show interaction with XDS exchanges? Current presumption is that this is not minimally needed, but likely would be a future need. Those exchanges that want to be XDS based already have a solution in MHD. The goal of this profile is to provide a FHIR stack without XDS or HL7 v2 backend. Thus the only interaction one might see in the future is an XCA interface to this MHDS.</t>
-  </si>
-  <si>
-    <t>Can Document Author be recorded as a link to data in the mCSD managed Directory, or must it continue to be mandated to be ‘contained’? Clearly it can be included as contained but is this still a mandate when the Organization and Practitioner are known to be managed. ***</t>
-  </si>
-  <si>
-    <t>This profile includes an option that allows the Document Registry to authorize the use of References where MHD forces contained. The necessary change to MHD has not been done yet in order to get feed back from Public Comment.</t>
-  </si>
-  <si>
-    <t>Can sourcePatientInfo be a version specific link to the centrally managed (PMIR) identity? Clearly it can continue to be contained but is this still a mandate when the Patient is known to be managed.***</t>
-  </si>
-  <si>
-    <t>There seems to be feedback that the need identified in XDS for sourcePatientInfo has not been important. Many exchanges recommend this element be left empty as one either has good control of patient identity. If one doesn’t have good control, the sourcePatientInfo element is only going to add to the confusion.</t>
-  </si>
-  <si>
-    <t>As diagrammed here there is no formal Document Repository, although the functionality is provided virtually. That is that a Document Source can choose to not include the document as a Binary resource, but rather include a URL to a repository that is recognized as part of the trust domain. This distinction is available in MHD today, although it is not pointed out as such and thus not well known. The only value to creating a Document Repository is to define input transaction as different from output transaction. Specifically by defining a Document Repository we enable third-party Repository systems. A Document Repository could be supported as is today, but is not defined by IHE MHDS profile.</t>
-  </si>
-  <si>
-    <t>The Figure X.1-1 is a high-level picture of the overall solution. It is not typical picture for an IHE profile. This high-level picture is used in the appendix in more detail. Is there comments or recommendations on how to improve this diagram?</t>
-  </si>
-  <si>
     <t>Introduction</t>
   </si>
   <si>
@@ -3067,9 +3046,6 @@
     <t>will give more full layout of the material in X.1</t>
   </si>
   <si>
-    <t>should we remove this? I think it is not wrong.</t>
-  </si>
-  <si>
     <t>it is mentioned in X.1</t>
   </si>
   <si>
@@ -3083,6 +3059,12 @@
   </si>
   <si>
     <t>I can't come up with better language. Although PMIR maintains a golden identitity, it does support linking in your local identifers into that golden identity. I think this section might need careful re-read in light of current PMIR solution as it does have a cross-reference pattern from the original HIE white paper</t>
+  </si>
+  <si>
+    <t>The MHDS environment allows for some normally contained Resources be recorded as a link to data in the mCSD managed Directory or PMIR Patient Identity Manager. This is defined in the “UnContained Reference Option”. The necessary change to MHD has not been done yet in order to get feedback from Public Comment. CP-ITI-1200 will be updating MHD to add an UnContained Reference Option for this support</t>
+  </si>
+  <si>
+    <t>keep open issue to remind us that the HIE whitepaper might get updated to include MHD/S</t>
   </si>
 </sst>
 </file>
@@ -3182,7 +3164,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3204,6 +3186,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3317,7 +3305,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3352,12 +3340,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -3378,6 +3360,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3717,10 +3708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L74"/>
+  <dimension ref="A1:L70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B67" zoomScale="125" zoomScaleNormal="123" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="123" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3736,32 +3727,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
       <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:12" ht="269.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="21" t="s">
         <v>156</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7"/>
@@ -3786,7 +3777,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3816,286 +3807,324 @@
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16" t="s">
+        <v>192</v>
+      </c>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="E7" s="18">
+        <v>1</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16" t="s">
+        <v>194</v>
+      </c>
+      <c r="E8" s="18">
+        <v>2</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="E9" s="18">
+        <v>184</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16" t="s">
+        <v>201</v>
+      </c>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="18">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:12" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="2">
+        <v>140</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="7"/>
+      <c r="J12" s="16"/>
+      <c r="K12" s="16"/>
+      <c r="L12" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="2">
+        <v>294</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E14" s="2">
+        <v>300</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="7"/>
+      <c r="J14" s="16" t="s">
+        <v>211</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2">
+        <v>317</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="7"/>
+      <c r="J15" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="K5" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B7" s="16"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E7" s="20">
-        <v>1</v>
-      </c>
-      <c r="F7" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="L7" s="18"/>
-    </row>
-    <row r="8" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E8" s="20">
-        <v>2</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>197</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="L8" s="18"/>
-    </row>
-    <row r="9" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B9" s="16"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E9" s="20">
-        <v>3</v>
-      </c>
-      <c r="F9" s="19" t="s">
-        <v>198</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="L9" s="18"/>
-    </row>
-    <row r="10" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B10" s="16"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E10" s="20">
-        <v>4</v>
-      </c>
-      <c r="F10" s="19" t="s">
-        <v>200</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>201</v>
-      </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="L10" s="18"/>
-    </row>
-    <row r="11" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E11" s="20">
-        <v>5</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>202</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="L11" s="18"/>
-    </row>
-    <row r="12" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="B12" s="16"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="E12" s="20">
-        <v>6</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>203</v>
-      </c>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="21" t="s">
-        <v>196</v>
-      </c>
-      <c r="L12" s="18"/>
-    </row>
-    <row r="13" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="18" t="s">
-        <v>204</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="E13" s="20">
-        <v>184</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>207</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18" t="s">
-        <v>208</v>
-      </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="18" t="s">
+      <c r="K15" s="16"/>
+      <c r="L15" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="20">
-        <v>1</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19" t="s">
-        <v>210</v>
-      </c>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18" t="s">
-        <v>211</v>
-      </c>
-      <c r="K14" s="18"/>
-      <c r="L14" s="18" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:12" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>65</v>
       </c>
       <c r="B16" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
       <c r="D16" s="2" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E16" s="2">
-        <v>140</v>
+        <v>319</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I16" s="7"/>
-      <c r="J16" s="18"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J16" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>65</v>
       </c>
@@ -4106,30 +4135,28 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="E17" s="2">
-        <v>294</v>
+        <v>324</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I17" s="7"/>
-      <c r="J17" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="K17" s="18"/>
-      <c r="L17" s="18" t="s">
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>65</v>
       </c>
@@ -4140,28 +4167,28 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>158</v>
+        <v>72</v>
       </c>
       <c r="E18" s="2">
-        <v>300</v>
+        <v>327</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="2"/>
+        <v>79</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>81</v>
+      </c>
       <c r="H18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I18" s="7"/>
-      <c r="J18" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="K18" s="18"/>
-      <c r="L18" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J18" s="16"/>
+      <c r="K18" s="16"/>
+      <c r="L18" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>65</v>
       </c>
@@ -4175,27 +4202,27 @@
         <v>72</v>
       </c>
       <c r="E19" s="2">
-        <v>317</v>
+        <v>333</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I19" s="7"/>
-      <c r="J19" s="18" t="s">
-        <v>219</v>
-      </c>
-      <c r="K19" s="18"/>
-      <c r="L19" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J19" s="16" t="s">
+        <v>214</v>
+      </c>
+      <c r="K19" s="16"/>
+      <c r="L19" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>65</v>
       </c>
@@ -4206,27 +4233,25 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2">
-        <v>319</v>
+        <v>370</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I20" s="7"/>
-      <c r="J20" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="K20" s="18"/>
-      <c r="L20" s="18" t="s">
-        <v>216</v>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4240,28 +4265,28 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="E21" s="2">
-        <v>324</v>
+        <v>377</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I21" s="7"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="18"/>
-      <c r="L21" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="231" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>65</v>
       </c>
@@ -4272,28 +4297,30 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="E22" s="2">
-        <v>327</v>
+        <v>379</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I22" s="7"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="16" t="s">
+        <v>215</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>65</v>
       </c>
@@ -4304,30 +4331,28 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="E23" s="2">
-        <v>333</v>
+        <v>415</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="H23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I23" s="7"/>
-      <c r="J23" s="18" t="s">
-        <v>221</v>
-      </c>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>65</v>
       </c>
@@ -4338,28 +4363,28 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E24" s="2">
-        <v>370</v>
+        <v>421</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I24" s="7"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>65</v>
       </c>
@@ -4370,28 +4395,28 @@
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E25" s="2">
-        <v>377</v>
+        <v>427</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>85</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I25" s="7"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="231" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>65</v>
       </c>
@@ -4402,30 +4427,28 @@
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="E26" s="2">
-        <v>379</v>
+        <v>430</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I26" s="7"/>
-      <c r="J26" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18" t="s">
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>65</v>
       </c>
@@ -4439,25 +4462,25 @@
         <v>99</v>
       </c>
       <c r="E27" s="2">
-        <v>415</v>
+        <v>435</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I27" s="7"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>65</v>
       </c>
@@ -4468,28 +4491,28 @@
         <v>1</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E28" s="2">
-        <v>421</v>
+        <v>476</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I28" s="7"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="8" customFormat="1" ht="230.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>65</v>
       </c>
@@ -4500,28 +4523,29 @@
         <v>1</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E29" s="2">
-        <v>427</v>
-      </c>
-      <c r="F29" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>85</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I29" s="7"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18" t="s">
+      <c r="J29" s="16" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="16"/>
+      <c r="L29" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" s="8" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>65</v>
       </c>
@@ -4532,28 +4556,29 @@
         <v>1</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="E30" s="2">
-        <v>430</v>
+        <v>494</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>85</v>
+        <v>111</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="7"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="18"/>
-      <c r="L30" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="J30" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>65</v>
       </c>
@@ -4564,28 +4589,27 @@
         <v>1</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="E31" s="2">
-        <v>435</v>
+        <v>494</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>102</v>
+        <v>157</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I31" s="7"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="18"/>
-      <c r="L31" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="8" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>65</v>
       </c>
@@ -4595,29 +4619,28 @@
       <c r="C32" s="2">
         <v>1</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="E32" s="2">
-        <v>476</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>105</v>
+      <c r="D32" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E32" s="12">
+        <v>500</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>85</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I32" s="7"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" s="8" customFormat="1" ht="230.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" s="8" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>65</v>
       </c>
@@ -4627,30 +4650,28 @@
       <c r="C33" s="2">
         <v>1</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" s="2">
-        <v>486</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>85</v>
+      <c r="D33" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="11">
+        <v>503</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J33" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" s="8" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" s="8" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>65</v>
       </c>
@@ -4661,29 +4682,27 @@
         <v>1</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E34" s="2">
-        <v>494</v>
+        <v>522</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J34" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="J34" s="16"/>
+      <c r="K34" s="16"/>
+      <c r="L34" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>65</v>
       </c>
@@ -4694,27 +4713,27 @@
         <v>1</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="E35" s="2">
-        <v>494</v>
+        <v>533</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>157</v>
+        <v>102</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" s="8" customFormat="1" ht="64.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J35" s="16"/>
+      <c r="K35" s="16"/>
+      <c r="L35" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>65</v>
       </c>
@@ -4724,28 +4743,28 @@
       <c r="C36" s="2">
         <v>1</v>
       </c>
-      <c r="D36" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="12">
-        <v>500</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>85</v>
+      <c r="D36" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="2">
+        <v>539</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="H36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" s="8" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J36" s="16"/>
+      <c r="K36" s="16"/>
+      <c r="L36" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" s="8" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>65</v>
       </c>
@@ -4755,28 +4774,28 @@
       <c r="C37" s="2">
         <v>1</v>
       </c>
-      <c r="D37" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="E37" s="11">
-        <v>503</v>
-      </c>
-      <c r="F37" s="11" t="s">
-        <v>115</v>
+      <c r="D37" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="2">
+        <v>542</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" s="8" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J37" s="16"/>
+      <c r="K37" s="16"/>
+      <c r="L37" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" s="8" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>65</v>
       </c>
@@ -4790,21 +4809,21 @@
         <v>119</v>
       </c>
       <c r="E38" s="2">
-        <v>522</v>
+        <v>551</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>120</v>
+        <v>125</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>126</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J38" s="18"/>
-      <c r="K38" s="18"/>
-      <c r="L38" s="18" t="s">
-        <v>216</v>
+      <c r="J38" s="16"/>
+      <c r="K38" s="16"/>
+      <c r="L38" s="16" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="39" spans="1:12" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
@@ -4818,27 +4837,27 @@
         <v>1</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E39" s="2">
-        <v>533</v>
+        <v>573</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="18"/>
-      <c r="K39" s="18"/>
-      <c r="L39" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+      <c r="L39" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>65</v>
       </c>
@@ -4849,27 +4868,27 @@
         <v>1</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E40" s="2">
-        <v>539</v>
+        <v>589</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>66</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J40" s="18"/>
-      <c r="K40" s="18"/>
-      <c r="L40" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" s="8" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="8" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>65</v>
       </c>
@@ -4880,27 +4899,29 @@
         <v>1</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E41" s="2">
-        <v>542</v>
+        <v>602</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>124</v>
+        <v>66</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>179</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J41" s="18"/>
-      <c r="K41" s="18"/>
-      <c r="L41" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" s="8" customFormat="1" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J41" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="K41" s="16"/>
+      <c r="L41" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="8" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>65</v>
       </c>
@@ -4911,27 +4932,29 @@
         <v>1</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E42" s="2">
-        <v>551</v>
+        <v>603</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>126</v>
+        <v>85</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J42" s="18"/>
-      <c r="K42" s="18"/>
-      <c r="L42" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="8" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J42" s="16" t="s">
+        <v>219</v>
+      </c>
+      <c r="K42" s="16"/>
+      <c r="L42" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>65</v>
       </c>
@@ -4942,24 +4965,26 @@
         <v>1</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="E43" s="2">
-        <v>573</v>
-      </c>
-      <c r="F43" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>128</v>
+        <v>613</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>97</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J43" s="18"/>
-      <c r="K43" s="18"/>
-      <c r="L43" s="18" t="s">
-        <v>216</v>
+      <c r="J43" s="18">
+        <v>51</v>
+      </c>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4973,27 +4998,27 @@
         <v>1</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="E44" s="2">
-        <v>589</v>
+        <v>613</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>131</v>
+        <v>95</v>
       </c>
       <c r="H44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J44" s="18"/>
-      <c r="K44" s="18"/>
-      <c r="L44" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" s="8" customFormat="1" ht="77.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J44" s="16"/>
+      <c r="K44" s="16"/>
+      <c r="L44" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" s="8" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>65</v>
       </c>
@@ -5004,29 +5029,27 @@
         <v>1</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>129</v>
+        <v>93</v>
       </c>
       <c r="E45" s="2">
-        <v>602</v>
+        <v>613</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G45" s="11" t="s">
-        <v>179</v>
+        <v>92</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="H45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J45" s="18" t="s">
-        <v>225</v>
-      </c>
-      <c r="K45" s="18"/>
-      <c r="L45" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" s="8" customFormat="1" ht="90" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J45" s="16"/>
+      <c r="K45" s="16"/>
+      <c r="L45" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" s="8" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>65</v>
       </c>
@@ -5036,30 +5059,30 @@
       <c r="C46" s="2">
         <v>1</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E46" s="2">
-        <v>603</v>
+      <c r="D46" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E46" s="11">
+        <v>620</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>85</v>
+        <v>134</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J46" s="18" t="s">
-        <v>226</v>
-      </c>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="K46" s="16"/>
+      <c r="L46" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>65</v>
       </c>
@@ -5069,30 +5092,31 @@
       <c r="C47" s="2">
         <v>1</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E47" s="2">
-        <v>613</v>
-      </c>
-      <c r="F47" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="G47" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J47" s="20">
-        <v>51</v>
-      </c>
-      <c r="K47" s="18"/>
-      <c r="L47" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="8" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E47" s="11">
+        <v>625</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="H47" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I47" s="7"/>
+      <c r="J47" s="16" t="s">
+        <v>221</v>
+      </c>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="141.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>65</v>
       </c>
@@ -5102,28 +5126,31 @@
       <c r="C48" s="2">
         <v>1</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E48" s="2">
-        <v>613</v>
+      <c r="D48" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" s="11">
+        <v>649</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="8" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="G48" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I48" s="7"/>
+      <c r="J48" s="16"/>
+      <c r="K48" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="L48" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>65</v>
       </c>
@@ -5133,28 +5160,29 @@
       <c r="C49" s="2">
         <v>1</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E49" s="2">
-        <v>613</v>
+      <c r="D49" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="E49" s="11">
+        <v>675</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G49" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H49" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>180</v>
+      </c>
+      <c r="H49" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J49" s="18"/>
-      <c r="K49" s="18"/>
-      <c r="L49" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="8" customFormat="1" ht="51.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="7"/>
+      <c r="J49" s="16"/>
+      <c r="K49" s="16"/>
+      <c r="L49" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>65</v>
       </c>
@@ -5165,29 +5193,28 @@
         <v>1</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="E50" s="11">
-        <v>620</v>
+        <v>710</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="H50" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="H50" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J50" s="18" t="s">
-        <v>227</v>
-      </c>
-      <c r="K50" s="18"/>
-      <c r="L50" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I50" s="7"/>
+      <c r="J50" s="16"/>
+      <c r="K50" s="16"/>
+      <c r="L50" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="282" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>65</v>
       </c>
@@ -5198,30 +5225,30 @@
         <v>1</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E51" s="11">
-        <v>625</v>
+        <v>726</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I51" s="7"/>
-      <c r="J51" s="18" t="s">
-        <v>228</v>
-      </c>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" ht="141.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J51" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>65</v>
       </c>
@@ -5232,26 +5259,26 @@
         <v>1</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="E52" s="11">
-        <v>649</v>
+        <v>820</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>104</v>
+        <v>182</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I52" s="7"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="21" t="s">
-        <v>229</v>
-      </c>
-      <c r="L52" s="18"/>
+      <c r="J52" s="16"/>
+      <c r="K52" s="16"/>
+      <c r="L52" s="16" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="53" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
@@ -5264,28 +5291,28 @@
         <v>1</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="E53" s="11">
-        <v>675</v>
+        <v>892</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="G53" s="11" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H53" s="11" t="s">
         <v>8</v>
       </c>
       <c r="I53" s="7"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>65</v>
       </c>
@@ -5296,28 +5323,30 @@
         <v>1</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="E54" s="11">
-        <v>710</v>
+        <v>894</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="G54" s="11" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I54" s="7"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="18"/>
-      <c r="L54" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="282" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J54" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="K54" s="16"/>
+      <c r="L54" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="39" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>65</v>
       </c>
@@ -5327,31 +5356,29 @@
       <c r="C55" s="2">
         <v>1</v>
       </c>
-      <c r="D55" s="11" t="s">
-        <v>144</v>
+      <c r="D55" s="2" t="s">
+        <v>153</v>
       </c>
       <c r="E55" s="11">
-        <v>726</v>
+        <v>1005</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>181</v>
+        <v>154</v>
+      </c>
+      <c r="G55" s="11" t="s">
+        <v>149</v>
       </c>
       <c r="H55" s="11" t="s">
         <v>8</v>
       </c>
       <c r="I55" s="7"/>
-      <c r="J55" s="18" t="s">
-        <v>230</v>
-      </c>
-      <c r="K55" s="18"/>
-      <c r="L55" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J55" s="16"/>
+      <c r="K55" s="23"/>
+      <c r="L55" s="16" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>65</v>
       </c>
@@ -5361,29 +5388,29 @@
       <c r="C56" s="2">
         <v>1</v>
       </c>
-      <c r="D56" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E56" s="11">
-        <v>820</v>
-      </c>
+      <c r="D56" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E56" s="11"/>
       <c r="F56" s="2" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="H56" s="11" t="s">
         <v>8</v>
       </c>
       <c r="I56" s="7"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="18"/>
-      <c r="L56" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J56" s="16"/>
+      <c r="K56" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="L56" s="16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>65</v>
       </c>
@@ -5394,28 +5421,30 @@
         <v>1</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="E57" s="11">
-        <v>892</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>146</v>
+        <v>1015</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H57" s="11" t="s">
         <v>8</v>
       </c>
       <c r="I57" s="7"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="18"/>
-      <c r="L57" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J57" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="K57" s="16"/>
+      <c r="L57" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>65</v>
       </c>
@@ -5426,30 +5455,28 @@
         <v>1</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E58" s="11">
-        <v>894</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="G58" s="11" t="s">
-        <v>162</v>
+        <v>1089</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>185</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I58" s="7"/>
-      <c r="J58" s="18" t="s">
-        <v>231</v>
-      </c>
-      <c r="K58" s="18"/>
-      <c r="L58" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J58" s="16"/>
+      <c r="K58" s="16"/>
+      <c r="L58" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>65</v>
       </c>
@@ -5459,29 +5486,28 @@
       <c r="C59" s="2">
         <v>1</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>153</v>
+      <c r="D59" s="11" t="s">
+        <v>166</v>
       </c>
       <c r="E59" s="11">
-        <v>1005</v>
+        <v>1288</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G59" s="11" t="s">
-        <v>149</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="G59" s="11"/>
       <c r="H59" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="21" t="s">
-        <v>232</v>
-      </c>
-      <c r="L59" s="18"/>
-    </row>
-    <row r="60" spans="1:12" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J59" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="K59" s="16"/>
+      <c r="L59" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>65</v>
       </c>
@@ -5491,29 +5517,28 @@
       <c r="C60" s="2">
         <v>1</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E60" s="11"/>
+      <c r="D60" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E60" s="11">
+        <v>1493</v>
+      </c>
       <c r="F60" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G60" s="11" t="s">
-        <v>152</v>
+        <v>169</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="H60" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I60" s="7"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18" t="s">
-        <v>233</v>
-      </c>
-      <c r="L60" s="18" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" ht="116.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J60" s="16"/>
+      <c r="K60" s="16"/>
+      <c r="L60" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>65</v>
       </c>
@@ -5524,30 +5549,29 @@
         <v>1</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="E61" s="11">
-        <v>1015</v>
-      </c>
-      <c r="F61" s="11" t="s">
-        <v>155</v>
+        <v>1498</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="H61" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I61" s="7"/>
-      <c r="J61" s="18" t="s">
-        <v>235</v>
-      </c>
-      <c r="K61" s="18"/>
-      <c r="L61" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J61" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="K61" s="16"/>
+      <c r="L61" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>65</v>
       </c>
@@ -5558,28 +5582,25 @@
         <v>1</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="E62" s="11">
-        <v>1089</v>
-      </c>
-      <c r="F62" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>185</v>
-      </c>
+        <v>1533</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="G62" s="11"/>
       <c r="H62" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I62" s="7"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="18"/>
-      <c r="L62" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" ht="103.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J62" s="16"/>
+      <c r="K62" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="L62" s="16"/>
+    </row>
+    <row r="63" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>65</v>
       </c>
@@ -5590,27 +5611,27 @@
         <v>1</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="E63" s="11">
-        <v>1288</v>
+        <v>1555</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G63" s="11"/>
+        <v>175</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>177</v>
+      </c>
       <c r="H63" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J63" s="18" t="s">
-        <v>236</v>
-      </c>
-      <c r="K63" s="18"/>
-      <c r="L63" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" ht="77.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J63" s="16"/>
+      <c r="K63" s="16"/>
+      <c r="L63" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>65</v>
       </c>
@@ -5621,151 +5642,67 @@
         <v>1</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E64" s="11">
-        <v>1493</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>169</v>
+        <v>1565</v>
+      </c>
+      <c r="F64" s="11" t="s">
+        <v>178</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H64" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="J64" s="18"/>
-      <c r="K64" s="18"/>
-      <c r="L64" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B65" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C65" s="2">
-        <v>1</v>
-      </c>
-      <c r="D65" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="E65" s="11">
-        <v>1498</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="G65" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="H65" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J65" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="K65" s="18"/>
-      <c r="L65" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="409.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B66" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C66" s="2">
-        <v>1</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="E66" s="11">
-        <v>1533</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J66" s="18"/>
-      <c r="K66" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="L66" s="18"/>
-    </row>
-    <row r="67" spans="1:12" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C67" s="2">
-        <v>1</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E67" s="11">
-        <v>1555</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="H67" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J67" s="18"/>
-      <c r="K67" s="18"/>
-      <c r="L67" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" ht="102.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B68" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C68" s="2">
-        <v>1</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E68" s="11">
-        <v>1565</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="H68" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="J68" s="18"/>
-      <c r="K68" s="18"/>
-      <c r="L68" s="18" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J64" s="16"/>
+      <c r="K64" s="16"/>
+      <c r="L64" s="16" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="13"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="13"/>
       <c r="C69" s="1"/>
@@ -5775,9 +5712,9 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
-      <c r="B70" s="13"/>
+      <c r="B70" s="3"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -5785,56 +5722,16 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H175:H179" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H171:H175" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Priority Names.A1-3"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H16:H174" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H12:H170" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>PriorityNames</formula1>
     </dataValidation>
   </dataValidations>
@@ -5847,7 +5744,7 @@
           <x14:formula1>
             <xm:f>'Supplement Names'!$A$1:$A$53</xm:f>
           </x14:formula1>
-          <xm:sqref>B16:B74</xm:sqref>
+          <xm:sqref>B12:B70</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>